<commit_message>
Fix set max budget bug
</commit_message>
<xml_diff>
--- a/Holiday Recommendations/cities.xlsx
+++ b/Holiday Recommendations/cities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ioana\Documents\UiPath\Holiday Recommendations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ioana\Desktop\RPA-UiPath\Holiday-Recommendations\Holiday Recommendations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -92,7 +92,7 @@
     <t>Abu Dhabi</t>
   </si>
   <si>
-    <t>Bucharest</t>
+    <t>Palma de Mallorca</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +514,7 @@
         <v>4</v>
       </c>
       <c r="E3">
-        <v>1456</v>
+        <v>3000</v>
       </c>
       <c r="F3">
         <v>2</v>

</xml_diff>